<commit_message>
add stock reports data
</commit_message>
<xml_diff>
--- a/invest/电力/电力.xlsx
+++ b/invest/电力/电力.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="全国" sheetId="5" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="营业收入_利润" sheetId="1" r:id="rId3"/>
     <sheet name="销售量" sheetId="2" r:id="rId4"/>
     <sheet name="研发投入" sheetId="3" r:id="rId5"/>
+    <sheet name="2016四大发电集团" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="60">
   <si>
     <t>近五年营业收入、利润</t>
   </si>
@@ -202,6 +203,34 @@
   <si>
     <t>装机变化</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>总用电亿千瓦时</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>亿千瓦时</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>华能</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>华电</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>国电</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>国电投</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Total</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -209,9 +238,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="180" formatCode="#,##0_ "/>
+    <numFmt numFmtId="176" formatCode="#,##0_ "/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +276,13 @@
       <name val="黑体"/>
       <family val="3"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -295,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -317,7 +353,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1004,11 +1049,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="77131776"/>
-        <c:axId val="77133312"/>
+        <c:axId val="47182592"/>
+        <c:axId val="47184128"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77131776"/>
+        <c:axId val="47182592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,7 +1063,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77133312"/>
+        <c:crossAx val="47184128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1026,7 +1071,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77133312"/>
+        <c:axId val="47184128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,7 +1082,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77131776"/>
+        <c:crossAx val="47182592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1299,11 +1344,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="77165696"/>
-        <c:axId val="77167232"/>
+        <c:axId val="47820800"/>
+        <c:axId val="47822336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77165696"/>
+        <c:axId val="47820800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1312,7 +1357,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77167232"/>
+        <c:crossAx val="47822336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1320,7 +1365,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77167232"/>
+        <c:axId val="47822336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1331,7 +1376,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77165696"/>
+        <c:crossAx val="47820800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1596,11 +1641,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="77515008"/>
-        <c:axId val="77520896"/>
+        <c:axId val="47592192"/>
+        <c:axId val="47593728"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77515008"/>
+        <c:axId val="47592192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,7 +1655,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77520896"/>
+        <c:crossAx val="47593728"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1618,7 +1663,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77520896"/>
+        <c:axId val="47593728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1629,7 +1674,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77515008"/>
+        <c:crossAx val="47592192"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2179,8 +2224,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B50" sqref="B45:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3472,4 +3517,110 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B3" s="16"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="17">
+        <v>59198</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B4" s="16"/>
+      <c r="C4" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="16"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B5" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="17">
+        <v>6108</v>
+      </c>
+      <c r="D5" s="18">
+        <f>C5/$D$3</f>
+        <v>0.10317916145815736</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B6" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="17">
+        <v>4919</v>
+      </c>
+      <c r="D6" s="18">
+        <f t="shared" ref="D6:D8" si="0">C6/$D$3</f>
+        <v>8.3094023446738066E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B7" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="17">
+        <v>5052</v>
+      </c>
+      <c r="D7" s="18">
+        <f t="shared" si="0"/>
+        <v>8.5340720970303055E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B8" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="17">
+        <v>3969</v>
+      </c>
+      <c r="D8" s="18">
+        <f t="shared" si="0"/>
+        <v>6.7046183992702457E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B9" s="16"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="16"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B10" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="17">
+        <f>SUM(C5:C8)</f>
+        <v>20048</v>
+      </c>
+      <c r="D10" s="18">
+        <f>SUM(D5:D8)</f>
+        <v>0.33866008986790092</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>